<commit_message>
Changes to TrancheBounds sheet
Changed name of TrancheBounds sheet to TrancheDetails and added Mean Gas Rates.
</commit_message>
<xml_diff>
--- a/MeanEmissionsFactorsByTranche.xlsx
+++ b/MeanEmissionsFactorsByTranche.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/tblackfd_mit_edu/Documents/SDM/Thesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{81B31D90-FB09-C143-BD7F-A13721D4AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5C85B69-0597-C643-A866-B2A3C18F48BF}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{81B31D90-FB09-C143-BD7F-A13721D4AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0CA58EB-C5B8-B442-A31E-835C853F37A2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" activeTab="1" xr2:uid="{4E2EA2BE-306F-4149-89F5-388E1A073B9F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Mean</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Equipment No</t>
+  </si>
+  <si>
+    <t>Mean Gas Rate</t>
   </si>
 </sst>
 </file>
@@ -1157,13 +1160,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795B8A72-C1BF-AB4A-8620-67223ED28960}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1279,6 +1285,41 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>3.3141656254018852E-3</v>
+      </c>
+      <c r="C4">
+        <v>2.3229257753825928E-2</v>
+      </c>
+      <c r="D4">
+        <v>6.0885670409754518E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.12176465229150621</v>
+      </c>
+      <c r="F4">
+        <v>0.27712243647722223</v>
+      </c>
+      <c r="G4">
+        <v>0.58810554596876741</v>
+      </c>
+      <c r="H4">
+        <v>1.787091075755936</v>
+      </c>
+      <c r="I4">
+        <v>5.7882521336484194</v>
+      </c>
+      <c r="J4">
+        <v>20.990273004878844</v>
+      </c>
+      <c r="K4">
+        <v>161.06811496813148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to TrancheDetails Sheet
Changed name of Mean Gas Rate row to "Normalised Gas Rate".
</commit_message>
<xml_diff>
--- a/MeanEmissionsFactorsByTranche.xlsx
+++ b/MeanEmissionsFactorsByTranche.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/tblackfd_mit_edu/Documents/SDM/Thesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{81B31D90-FB09-C143-BD7F-A13721D4AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0CA58EB-C5B8-B442-A31E-835C853F37A2}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{81B31D90-FB09-C143-BD7F-A13721D4AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{532EB741-D2B5-C647-8B84-BE139318ABAB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" activeTab="1" xr2:uid="{4E2EA2BE-306F-4149-89F5-388E1A073B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="EmissionsFactors" sheetId="1" r:id="rId1"/>
-    <sheet name="TrancheBounds" sheetId="2" r:id="rId2"/>
+    <sheet name="TrancheDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" iterate="1"/>
   <extLst>
@@ -108,7 +108,7 @@
     <t>Equipment No</t>
   </si>
   <si>
-    <t>Mean Gas Rate</t>
+    <t>Normalised Gas Rate</t>
   </si>
 </sst>
 </file>
@@ -1163,12 +1163,12 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change to TrancheDetails sheet
Added row for "Frac Total Gas", taken directly from OPGEE.
</commit_message>
<xml_diff>
--- a/MeanEmissionsFactorsByTranche.xlsx
+++ b/MeanEmissionsFactorsByTranche.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/tblackfd_mit_edu/Documents/SDM/Thesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{81B31D90-FB09-C143-BD7F-A13721D4AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{532EB741-D2B5-C647-8B84-BE139318ABAB}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{81B31D90-FB09-C143-BD7F-A13721D4AC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F999A6FD-BAE4-6847-8E90-4B487C15E8FE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" activeTab="1" xr2:uid="{4E2EA2BE-306F-4149-89F5-388E1A073B9F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Mean</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Normalised Gas Rate</t>
+  </si>
+  <si>
+    <t>Frac Total Gas</t>
   </si>
 </sst>
 </file>
@@ -1160,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795B8A72-C1BF-AB4A-8620-67223ED28960}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1320,6 +1323,41 @@
         <v>161.06811496813148</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>2.9534195905716725E-4</v>
+      </c>
+      <c r="C5">
+        <v>3.6453349502072671E-3</v>
+      </c>
+      <c r="D5">
+        <v>6.6109069432481451E-3</v>
+      </c>
+      <c r="E5">
+        <v>1.5144015324681041E-2</v>
+      </c>
+      <c r="F5">
+        <v>5.6319634110065388E-2</v>
+      </c>
+      <c r="G5">
+        <v>7.8406143359654346E-2</v>
+      </c>
+      <c r="H5">
+        <v>0.25340652577454159</v>
+      </c>
+      <c r="I5">
+        <v>0.1311533569343277</v>
+      </c>
+      <c r="J5">
+        <v>0.4145126613663031</v>
+      </c>
+      <c r="K5">
+        <v>4.0506079277914275E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>